<commit_message>
Release to TI ITI.FAIS
</commit_message>
<xml_diff>
--- a/ITI/FAIS/StructureDefinition-IHE.FAIS.Audit.Claim.Cancel.xlsx
+++ b/ITI/FAIS/StructureDefinition-IHE.FAIS.Audit.Claim.Cancel.xlsx
@@ -33,7 +33,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.0.0-comment</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-07T10:12:51-05:00</t>
+    <t>2024-11-13T10:59:36-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -573,15 +573,15 @@
     <t>https://profiles.ihe.net/ITI/BALP/ValueSet/AllUpdateVS</t>
   </si>
   <si>
-    <t>AuditEvent.subtype:itiYY8</t>
-  </si>
-  <si>
-    <t>itiYY8</t>
+    <t>AuditEvent.subtype:iti127</t>
+  </si>
+  <si>
+    <t>iti127</t>
   </si>
   <si>
     <t>&lt;valueCoding xmlns="http://hl7.org/fhir"&gt;
   &lt;system value="urn:ihe:event-type-code"/&gt;
-  &lt;code value="ITI-YY8"/&gt;
+  &lt;code value="ITI-127"/&gt;
   &lt;display value="Cancel Claim"/&gt;
 &lt;/valueCoding&gt;</t>
   </si>

</xml_diff>